<commit_message>
Fix Encrypt / Hash
</commit_message>
<xml_diff>
--- a/App_TestWithdrawFund/test.xlsx
+++ b/App_TestWithdrawFund/test.xlsx
@@ -3,22 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CPU01661-local\Documents\GitHub\ToolTestWithdrawFund\App_TestWithdrawFund\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="url" sheetId="2" r:id="rId1"/>
-    <sheet name="api_inquireCard" sheetId="3" r:id="rId2"/>
-    <sheet name="api_withdraw" sheetId="4" r:id="rId3"/>
+    <sheet name="hash_data" sheetId="5" r:id="rId2"/>
+    <sheet name="api_inquireCard" sheetId="3" r:id="rId3"/>
+    <sheet name="demo" sheetId="6" r:id="rId4"/>
+    <sheet name="api_withdraw" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="44">
   <si>
     <t>STT</t>
   </si>
@@ -38,12 +40,6 @@
   </si>
   <si>
     <t>TestCase</t>
-  </si>
-  <si>
-    <t>tid</t>
-  </si>
-  <si>
-    <t>amt</t>
   </si>
   <si>
     <t>T160712KWQZ09Q8S</t>
@@ -91,9 +87,6 @@
     <t>Result Real</t>
   </si>
   <si>
-    <t>chksum</t>
-  </si>
-  <si>
     <t>signature</t>
   </si>
   <si>
@@ -124,21 +117,56 @@
     <t>100000</t>
   </si>
   <si>
-    <t>a7</t>
+    <t>Name Data</t>
   </si>
   <si>
-    <t>100</t>
+    <t>Category Hash</t>
   </si>
   <si>
-    <t>a8</t>
+    <t>AES-256</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>Kgnk3cpOwDVAtdNfWJ21cCNs3P4IGy81</t>
+  </si>
+  <si>
+    <t>Kgnk3cpOwDVAtdNf</t>
+  </si>
+  <si>
+    <t>chksum-SHA-256</t>
+  </si>
+  <si>
+    <t>a15</t>
+  </si>
+  <si>
+    <t>a16</t>
+  </si>
+  <si>
+    <t>demo</t>
+  </si>
+  <si>
+    <t>http://mi-payment-sandbox.123pay.vn/getBank</t>
+  </si>
+  <si>
+    <t>TRUSTPAY</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>1472035434447</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +178,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,10 +208,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -211,8 +248,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -491,96 +531,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="41.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="60.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="81.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="60" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="81" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M707"/>
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="8" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+      <formula1>"AES-256, RC-4, AES-512"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M707"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -597,23 +691,23 @@
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -622,15 +716,15 @@
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
@@ -644,13 +738,13 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
@@ -659,41 +753,39 @@
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
+      <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="K4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="7" t="n">
-        <v>1.0</v>
+        <v>21</v>
+      </c>
+      <c r="L4" s="7">
+        <v>5000</v>
       </c>
       <c r="M4" t="b">
         <f>IF(K4&lt;&gt;"",IF(K4  = L4,TRUE, FALSE),"")</f>
@@ -706,33 +798,35 @@
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="K5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1</v>
+      </c>
       <c r="M5" t="b">
         <f t="shared" ref="M5:M23" si="0">IF(K5&lt;&gt;"",IF(K5  = L5,TRUE, FALSE),"")</f>
         <v>0</v>
@@ -1033,6 +1127,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
+      <c r="I24" s="4"/>
       <c r="L24" s="2"/>
       <c r="M24" t="str">
         <f t="shared" ref="M24:M44" si="1">IF(K24&lt;&gt;"",IF(K24=L24,TRUE,FALSE),"")</f>
@@ -1041,6 +1136,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
+      <c r="I25" s="4"/>
       <c r="L25" s="2"/>
       <c r="M25" t="str">
         <f t="shared" si="1"/>
@@ -1049,6 +1145,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
+      <c r="I26" s="4"/>
       <c r="L26" s="2"/>
       <c r="M26" t="str">
         <f t="shared" si="1"/>
@@ -5800,8 +5897,8 @@
     <mergeCell ref="I2:I3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I21">
-      <formula1>"chksum, signature, no"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I26">
+      <formula1>"chksum-SHA-1, chksum-SHA-256, chksum-SHA-512, chksum-MD5, signature, no"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5809,26 +5906,159 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H3"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4">
+      <formula1>"chksum-SHA-1, chksum-SHA-256, chksum-SHA-512, chksum-MD5, signature, no"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection sqref="A1:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="2" max="2" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -5845,22 +6075,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -5869,14 +6099,14 @@
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
@@ -5890,10 +6120,10 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -5902,29 +6132,26 @@
       <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G4">
         <v>10000</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -5932,8 +6159,8 @@
       <c r="J4" s="8">
         <v>1</v>
       </c>
-      <c r="K4" s="8" t="n">
-        <v>0.0</v>
+      <c r="K4" s="8">
+        <v>6100</v>
       </c>
       <c r="L4" t="b">
         <f xml:space="preserve"> IF(J4 &lt;&gt; "",  IF(J4 = K4, TRUE, FALSE), "")</f>
@@ -5945,30 +6172,32 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="G5">
         <v>100000</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I5">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="J5" s="8">
         <v>1</v>
       </c>
-      <c r="K5" s="8"/>
+      <c r="K5" s="8">
+        <v>1</v>
+      </c>
       <c r="L5" t="b">
         <f t="shared" ref="L5:L68" si="0">IF(J5&lt;&gt;"",IF(J5=K5,TRUE,FALSE),"")</f>
         <v>0</v>
@@ -6589,11 +6818,15 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="J1:J3"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H86">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H30:H86">
       <formula1>"chksum, signature, no"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H29">
+      <formula1>"chksum-SHA-1, chksum-SHA-256, chksum-SHA-512, chksum-MD5, signature, no"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>